<commit_message>
separate classifier script, some tuning esketit
</commit_message>
<xml_diff>
--- a/data/barriers.xlsx
+++ b/data/barriers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="696">
   <si>
     <t xml:space="preserve">group</t>
   </si>
@@ -1994,6 +1994,120 @@
   </si>
   <si>
     <t xml:space="preserve">16+1,2,3,4-tetrachlorocyclopropene Exo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 21, 24, 25, 32, 20, 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["c2","c4","c8","c6","c13","c10"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Br-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 21, 24, 25, 33, 20, 28 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Cl-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 22, 25, 26, 36, 21, 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-F-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 24, 27, 28, 36, 23, 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Me-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 23, 26, 27, 36, 22, 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-NH2-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 23, 26, 28, 35, 22, 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-OH-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 22, 25, 26, 34, 21, 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-SH-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,13,6,8,4,2, 24, 27, 28, 38, 33, 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-SiH3-syn-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 22, 25, 27, 36, 21, 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["c3","c5","c9","c7","c14","c11"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Br-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 22, 25, 26, 36, 21, 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Cl-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 22, 25, 26, 36, 19, 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-F-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 25, 28, 29, 39, 22, 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-Me-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 24, 27, 28, 38, 21, 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-NH2-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 23, 26, 27, 37, 20, 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-OH-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,13,7,9,5,3, 23, 26, 27, 36, 22, 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">["c3","c5","c9","c7","c13","c11"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-SH-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 25, 28, 29, 39, 24, 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-SiH3-anti-ethylene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,14,7,9,5,3, 23, 26, 28, 36, 22, 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5-H ethylene</t>
   </si>
 </sst>
 </file>
@@ -2166,7 +2280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2267,10 +2381,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2350,8 +2460,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A226" activeCellId="0" sqref="A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9162,14 +9272,498 @@
         <v>74.5676</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="25"/>
-    </row>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="25"/>
-    </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="25"/>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B233" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E233" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="F233" s="18" t="n">
+        <v>-2843.794424</v>
+      </c>
+      <c r="G233" s="18" t="n">
+        <v>-2843.760853</v>
+      </c>
+      <c r="H233" s="18" t="n">
+        <v>0.033571</v>
+      </c>
+      <c r="I233" s="18" t="n">
+        <v>88.1407</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B234" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E234" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="F234" s="18" t="n">
+        <v>-732.2803886</v>
+      </c>
+      <c r="G234" s="18" t="n">
+        <v>-732.2500126</v>
+      </c>
+      <c r="H234" s="18" t="n">
+        <v>0.030376</v>
+      </c>
+      <c r="I234" s="18" t="n">
+        <v>79.7522</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B235" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E235" s="19" t="s">
+        <v>665</v>
+      </c>
+      <c r="F235" s="18" t="n">
+        <v>-371.9123527</v>
+      </c>
+      <c r="G235" s="18" t="n">
+        <v>-371.888354</v>
+      </c>
+      <c r="H235" s="18" t="n">
+        <v>0.0239987</v>
+      </c>
+      <c r="I235" s="18" t="n">
+        <v>63.0086</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B236" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E236" s="19" t="s">
+        <v>667</v>
+      </c>
+      <c r="F236" s="18" t="n">
+        <v>-312.0045016</v>
+      </c>
+      <c r="G236" s="18" t="n">
+        <v>-311.9682761</v>
+      </c>
+      <c r="H236" s="18" t="n">
+        <v>0.0362255</v>
+      </c>
+      <c r="I236" s="18" t="n">
+        <v>95.1101</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B237" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E237" s="19" t="s">
+        <v>669</v>
+      </c>
+      <c r="F237" s="18" t="n">
+        <v>-328.0301972</v>
+      </c>
+      <c r="G237" s="18" t="n">
+        <v>-327.9978246</v>
+      </c>
+      <c r="H237" s="18" t="n">
+        <v>0.0323726</v>
+      </c>
+      <c r="I237" s="18" t="n">
+        <v>84.9943</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B238" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E238" s="19" t="s">
+        <v>671</v>
+      </c>
+      <c r="F238" s="18" t="n">
+        <v>-347.8957185</v>
+      </c>
+      <c r="G238" s="18" t="n">
+        <v>-347.8643236</v>
+      </c>
+      <c r="H238" s="18" t="n">
+        <v>0.0313949</v>
+      </c>
+      <c r="I238" s="18" t="n">
+        <v>82.4273</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B239" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E239" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="F239" s="18" t="n">
+        <v>-670.8706523</v>
+      </c>
+      <c r="G239" s="18" t="n">
+        <v>-670.8371049</v>
+      </c>
+      <c r="H239" s="18" t="n">
+        <v>0.0335474</v>
+      </c>
+      <c r="I239" s="18" t="n">
+        <v>88.0787</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B240" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E240" s="19" t="s">
+        <v>675</v>
+      </c>
+      <c r="F240" s="18" t="n">
+        <v>-563.3882448</v>
+      </c>
+      <c r="G240" s="18" t="n">
+        <v>-563.3431414</v>
+      </c>
+      <c r="H240" s="18" t="n">
+        <v>0.0451034</v>
+      </c>
+      <c r="I240" s="18" t="n">
+        <v>118.419</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B241" s="18" t="n">
+        <v>9</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E241" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="F241" s="18" t="n">
+        <v>-2843.793175</v>
+      </c>
+      <c r="G241" s="18" t="n">
+        <v>-2843.762039</v>
+      </c>
+      <c r="H241" s="18" t="n">
+        <v>0.0311361</v>
+      </c>
+      <c r="I241" s="18" t="n">
+        <v>81.7478</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B242" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E242" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="F242" s="18" t="n">
+        <v>-732.281414</v>
+      </c>
+      <c r="G242" s="18" t="n">
+        <v>-732.2499837</v>
+      </c>
+      <c r="H242" s="18" t="n">
+        <v>0.0314303</v>
+      </c>
+      <c r="I242" s="18" t="n">
+        <v>82.5203</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B243" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E243" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="F243" s="18" t="n">
+        <v>-371.9103278</v>
+      </c>
+      <c r="G243" s="18" t="n">
+        <v>-371.8795681</v>
+      </c>
+      <c r="H243" s="18" t="n">
+        <v>0.0307597</v>
+      </c>
+      <c r="I243" s="18" t="n">
+        <v>80.7596</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B244" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E244" s="19" t="s">
+        <v>684</v>
+      </c>
+      <c r="F244" s="18" t="n">
+        <v>-312.0042981</v>
+      </c>
+      <c r="G244" s="18" t="n">
+        <v>-311.9692874</v>
+      </c>
+      <c r="H244" s="18" t="n">
+        <v>0.0350107</v>
+      </c>
+      <c r="I244" s="18" t="n">
+        <v>91.9206</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B245" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E245" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="F245" s="18" t="n">
+        <v>-328.0286427</v>
+      </c>
+      <c r="G245" s="18" t="n">
+        <v>-327.9952322</v>
+      </c>
+      <c r="H245" s="18" t="n">
+        <v>0.0334105</v>
+      </c>
+      <c r="I245" s="18" t="n">
+        <v>87.7193</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B246" s="18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E246" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="F246" s="18" t="n">
+        <v>-347.8917703</v>
+      </c>
+      <c r="G246" s="18" t="n">
+        <v>-347.8604927</v>
+      </c>
+      <c r="H246" s="18" t="n">
+        <v>0.0312776</v>
+      </c>
+      <c r="I246" s="18" t="n">
+        <v>82.1193</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B247" s="18" t="n">
+        <v>15</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E247" s="19" t="s">
+        <v>691</v>
+      </c>
+      <c r="F247" s="18" t="n">
+        <v>-670.8733357</v>
+      </c>
+      <c r="G247" s="18" t="n">
+        <v>-670.8394733</v>
+      </c>
+      <c r="H247" s="18" t="n">
+        <v>0.0338624</v>
+      </c>
+      <c r="I247" s="18" t="n">
+        <v>88.9057</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B248" s="18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E248" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="F248" s="18" t="n">
+        <v>-563.3890265</v>
+      </c>
+      <c r="G248" s="18" t="n">
+        <v>-563.3526417</v>
+      </c>
+      <c r="H248" s="18" t="n">
+        <v>0.0363848</v>
+      </c>
+      <c r="I248" s="18" t="n">
+        <v>95.5283</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B249" s="18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E249" s="19" t="s">
+        <v>695</v>
+      </c>
+      <c r="F249" s="18" t="n">
+        <v>-272.6903599</v>
+      </c>
+      <c r="G249" s="18" t="n">
+        <v>-272.6567733</v>
+      </c>
+      <c r="H249" s="18" t="n">
+        <v>0.0335866</v>
+      </c>
+      <c r="I249" s="18" t="n">
+        <v>88.1816</v>
+      </c>
     </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>